<commit_message>
updated diapers_by_county and tn_us_diapers
</commit_message>
<xml_diff>
--- a/data/tennessee_diaper_facts.xlsx
+++ b/data/tennessee_diaper_facts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balle\Documents\NSS\projects\nashville_diaper_connection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642D93A2-342E-4C13-AC74-69BFECBD4704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C85E7E-A8CE-4D71-83C9-55559FF5157F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{4D52C39A-9E86-4B46-BC5E-67705CD94153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +32,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,4 +768,313 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA67B4F5-24EC-49C2-81FE-9A927204857B}">
+  <dimension ref="A1:AE3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="3" max="3" width="15.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1:AE3">TRANSPOSE(Sheet1!A1:'Sheet1'!C31)</f>
+        <v>US and Tennessee Diaper Facts - https://nationaldiaperbanknetwork.org/wp-content/uploads/2020/03/2019_State_Diaper_Facts_12_2019_Tennessee.pdf</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Total Population Under Age 3</v>
+      </c>
+      <c r="D1" t="str">
+        <v>% of children under age 18 are infants or toddlers</v>
+      </c>
+      <c r="E1" t="str">
+        <v>% Live in families earning less than 100% of FPL</v>
+      </c>
+      <c r="F1" t="str">
+        <v>% Live in families earning 100% to 200% of FPL</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Percentage of Births Covered by Medicaid</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Percentage of WIC Recipients that Are Infants</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Percentage of TANF Families with at Least One Child Under Age 3</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Percentage of SNAP Recipients Under Age 5</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Mothers with Infants in the Workforce</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Nationally, 57% of parents experiencing
+diaper need who rely on child care said
+they missed an average of four days of
+school or work in the past month because
+they didn't have diapers.</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Cost of Infant Care as a Percentage of Income - for all households nationwide</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Two-Parent Households</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Single-Parent Households</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1" t="str">
+        <v>Infants, toddlers, and mothers participate in Early Head Start</v>
+      </c>
+      <c r="V1" t="str">
+        <v>Children Under Age 3 Receiving Federal Child Support</v>
+      </c>
+      <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1" t="str">
+        <v>The only federal assistance program that can be used for diapers is TANF</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Max Benefit for Family of 3 (1 Parent &amp; 2 Children) - July, 2020</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Diaper Costs Compared to Benefit - 29%</v>
+      </c>
+      <c r="AA1">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Number of Diaper Banks - 5 donating 1,056,699</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>50 diapers per child per month</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Infants and toddlers helped monthly</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Diapers distributed annually</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A2" t="str">
+        <v>TN</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>241516</v>
+      </c>
+      <c r="D2">
+        <v>0.16</v>
+      </c>
+      <c r="E2">
+        <v>0.15</v>
+      </c>
+      <c r="F2">
+        <v>0.23</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.51</v>
+      </c>
+      <c r="I2">
+        <v>0.26</v>
+      </c>
+      <c r="J2">
+        <v>0.3</v>
+      </c>
+      <c r="K2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0.65</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0.12</v>
+      </c>
+      <c r="S2">
+        <v>0.4</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>2265</v>
+      </c>
+      <c r="V2">
+        <v>0.41</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>277</v>
+      </c>
+      <c r="Z2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>5</v>
+      </c>
+      <c r="AC2">
+        <v>80</v>
+      </c>
+      <c r="AD2">
+        <v>1761</v>
+      </c>
+      <c r="AE2">
+        <v>1056699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A3" t="str">
+        <v>US</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>11752545</v>
+      </c>
+      <c r="D3">
+        <v>0.16</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <v>0.22</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.43</v>
+      </c>
+      <c r="I3">
+        <v>0.23</v>
+      </c>
+      <c r="J3">
+        <v>0.32</v>
+      </c>
+      <c r="K3">
+        <v>0.13</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0.65</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.13</v>
+      </c>
+      <c r="S3">
+        <v>0.44</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>164739</v>
+      </c>
+      <c r="V3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>477</v>
+      </c>
+      <c r="Z3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>200</v>
+      </c>
+      <c r="AC3">
+        <v>80</v>
+      </c>
+      <c r="AD3">
+        <v>197000</v>
+      </c>
+      <c r="AE3">
+        <v>68000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>